<commit_message>
parse dynamic load cases
</commit_message>
<xml_diff>
--- a/ETABSImporter/Examples/Cartel1.xlsx
+++ b/ETABSImporter/Examples/Cartel1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\STKOPlugIns\ETABSImporter\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA2576B-CFA3-4EEA-8C0A-B43C926C1D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDE0190-AC83-49B7-8BCE-4522D2F58902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7AA3E9DA-AF88-4948-BDFB-D1D4C0EAF3A0}"/>
   </bookViews>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA5DCB6-0F24-4F20-A73F-B71DEE222F03}">
   <dimension ref="N1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="N7" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O1" t="s">
@@ -627,7 +627,7 @@
       </c>
     </row>
     <row r="5" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O5" t="s">
@@ -635,7 +635,7 @@
       </c>
     </row>
     <row r="6" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="O6" t="s">
@@ -643,7 +643,7 @@
       </c>
     </row>
     <row r="7" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O7" t="s">
@@ -689,7 +689,7 @@
       </c>
     </row>
     <row r="12" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="O12" t="s">
@@ -727,7 +727,7 @@
       </c>
     </row>
     <row r="16" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="O16">
@@ -735,7 +735,7 @@
       </c>
     </row>
     <row r="17" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="O17">
@@ -950,5 +950,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>